<commit_message>
Update SkillUI & Fixed Traning Scene Error
</commit_message>
<xml_diff>
--- a/Documents/SlashBash Character Skill Sheet.xlsx
+++ b/Documents/SlashBash Character Skill Sheet.xlsx
@@ -102,6 +102,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Original Attack 2, this is a consistent attack, have two damage, which means it will have 60 damage for now each is 30.</t>
     </r>
     <r>
@@ -819,6 +825,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Original Attack 2</t>
     </r>
     <r>
@@ -2290,9 +2302,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2171700</xdr:rowOff>
+      <xdr:colOff>699135</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2152650" cy="1028700"/>
     <xdr:pic>
@@ -2308,7 +2320,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9460865" y="3257550"/>
+          <a:off x="9317990" y="3305175"/>
           <a:ext cx="2152650" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3158,7 +3170,7 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7353300" cy="4152900"/>
+    <xdr:ext cx="7353300" cy="4114800"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="38" name="image46.png" title="Image"/>
@@ -3173,7 +3185,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5040630" y="13382625"/>
-          <a:ext cx="7353300" cy="4152900"/>
+          <a:ext cx="7353300" cy="4114800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3676,8 +3688,8 @@
   </sheetPr>
   <dimension ref="A1:AG993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -4201,7 +4213,7 @@
       <c r="AF10" s="12"/>
       <c r="AG10" s="12"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" ht="12.75" spans="1:33">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>

</xml_diff>